<commit_message>
first look @ kid data
</commit_message>
<xml_diff>
--- a/data/adult_baseline.xlsx
+++ b/data/adult_baseline.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/madelinemeyers/Documents/GitHub/iteratedlearning/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F674FCEF-326F-DD4C-9AE5-54F0A98DFFEB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADA25C60-60E0-6F4B-8D65-A60D151F6C85}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="60" windowWidth="27500" windowHeight="17440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="adult_baseline" sheetId="1" r:id="rId1"/>
     <sheet name="adult_baseline_full" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6958" uniqueCount="1647">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6955" uniqueCount="1648">
   <si>
     <t>unique_id</t>
   </si>
@@ -5694,6 +5694,9 @@
   <si>
     <t xml:space="preserve">1 0 0 0 0 0 0 0 0 0 1 1 0 0 0 0 0 0 0 0 0 1 1 0 0 0 0 0 0 0 0 0 0 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 1 0 0 0 0 0 1 0 0 0 1 0
 </t>
+  </si>
+  <si>
+    <t>thrown</t>
   </si>
 </sst>
 </file>
@@ -29503,8 +29506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BE195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="AI145" sqref="AI145"/>
+    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
+      <selection activeCell="BB182" sqref="BB182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -29512,11 +29515,12 @@
     <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="0" style="9" hidden="1" customWidth="1"/>
     <col min="8" max="10" width="0" style="9" hidden="1" customWidth="1"/>
+    <col min="19" max="53" width="0" hidden="1" customWidth="1"/>
     <col min="54" max="54" width="11" style="9" customWidth="1"/>
     <col min="55" max="16384" width="10.83203125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -29676,8 +29680,11 @@
       <c r="BA1" t="s">
         <v>1580</v>
       </c>
+      <c r="BB1" s="9" t="s">
+        <v>1647</v>
+      </c>
     </row>
-    <row r="2" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>66</v>
       </c>
@@ -29838,8 +29845,11 @@
         <f>SUM(AV2,AQ2,AL2,AG2,AB2,W2,R2,M2)</f>
         <v>0</v>
       </c>
+      <c r="BB2" s="9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>115</v>
       </c>
@@ -30000,8 +30010,11 @@
         <f t="shared" ref="BA3:BA67" si="0">SUM(AV3,AQ3,AL3,AG3,AB3,W3,R3,M3)</f>
         <v>72</v>
       </c>
+      <c r="BB3" s="9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>131</v>
       </c>
@@ -30162,8 +30175,11 @@
         <f t="shared" si="0"/>
         <v>91</v>
       </c>
+      <c r="BB4" s="9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>156</v>
       </c>
@@ -30324,8 +30340,11 @@
         <f t="shared" si="0"/>
         <v>97</v>
       </c>
+      <c r="BB5" s="9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>172</v>
       </c>
@@ -30486,8 +30505,11 @@
         <f t="shared" si="0"/>
         <v>114</v>
       </c>
+      <c r="BB6" s="9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>180</v>
       </c>
@@ -30648,8 +30670,11 @@
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
+      <c r="BB7" s="9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="8" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>184</v>
       </c>
@@ -30810,8 +30835,11 @@
         <f t="shared" si="0"/>
         <v>178</v>
       </c>
+      <c r="BB8" s="9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="9" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>212</v>
       </c>
@@ -30972,8 +31000,11 @@
         <f t="shared" si="0"/>
         <v>296</v>
       </c>
+      <c r="BB9" s="9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>1050</v>
       </c>
@@ -31132,8 +31163,11 @@
         <f t="shared" si="0"/>
         <v>177</v>
       </c>
+      <c r="BB10" s="9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="11" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
         <v>199</v>
       </c>
@@ -31294,8 +31328,11 @@
         <f t="shared" si="0"/>
         <v>81</v>
       </c>
+      <c r="BB11" s="9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="12" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>221</v>
       </c>
@@ -31456,8 +31493,11 @@
         <f t="shared" si="0"/>
         <v>71</v>
       </c>
+      <c r="BB12" s="9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="13" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>276</v>
       </c>
@@ -31618,8 +31658,11 @@
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
+      <c r="BB13" s="9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="14" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>386</v>
       </c>
@@ -31780,8 +31823,11 @@
         <f t="shared" si="0"/>
         <v>136</v>
       </c>
+      <c r="BB14" s="9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="15" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
         <v>462</v>
       </c>
@@ -31940,8 +31986,11 @@
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
+      <c r="BB15" s="9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="16" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
         <v>481</v>
       </c>
@@ -32102,8 +32151,11 @@
         <f t="shared" si="0"/>
         <v>122</v>
       </c>
+      <c r="BB16" s="9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="17" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
         <v>630</v>
       </c>
@@ -32264,8 +32316,11 @@
         <f t="shared" si="0"/>
         <v>235</v>
       </c>
+      <c r="BB17" s="9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="18" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
         <v>394</v>
       </c>
@@ -32426,8 +32481,11 @@
         <f t="shared" si="0"/>
         <v>83</v>
       </c>
+      <c r="BB18" s="9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="19" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
         <v>422</v>
       </c>
@@ -32588,8 +32646,11 @@
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
+      <c r="BB19" s="9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="20" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
         <v>547</v>
       </c>
@@ -32750,8 +32811,11 @@
         <f t="shared" si="0"/>
         <v>128</v>
       </c>
+      <c r="BB20" s="9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="21" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
         <v>735</v>
       </c>
@@ -32912,8 +32976,11 @@
         <f t="shared" si="0"/>
         <v>250</v>
       </c>
+      <c r="BB21" s="9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="22" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
         <v>848</v>
       </c>
@@ -33072,8 +33139,11 @@
         <f t="shared" si="0"/>
         <v>67</v>
       </c>
+      <c r="BB22" s="9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="23" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
         <v>514</v>
       </c>
@@ -33234,8 +33304,11 @@
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
+      <c r="BB23" s="9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="24" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
         <v>535</v>
       </c>
@@ -33396,8 +33469,11 @@
         <f t="shared" si="0"/>
         <v>67</v>
       </c>
+      <c r="BB24" s="9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="25" spans="1:53" s="20" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:54" s="20" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="20" t="s">
         <v>758</v>
       </c>
@@ -33558,8 +33634,11 @@
         <f t="shared" si="0"/>
         <v>405</v>
       </c>
+      <c r="BB25" s="20">
+        <v>1</v>
+      </c>
     </row>
-    <row r="26" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
         <v>653</v>
       </c>
@@ -33720,8 +33799,11 @@
         <f t="shared" si="0"/>
         <v>170</v>
       </c>
+      <c r="BB26" s="9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="27" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
         <v>1088</v>
       </c>
@@ -33880,8 +33962,11 @@
         <f t="shared" si="0"/>
         <v>117</v>
       </c>
+      <c r="BB27" s="9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="28" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
         <v>69</v>
       </c>
@@ -34043,7 +34128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
         <v>253</v>
       </c>
@@ -34205,7 +34290,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="30" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
         <v>408</v>
       </c>
@@ -34367,7 +34452,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="31" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
         <v>522</v>
       </c>
@@ -34529,7 +34614,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="32" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
         <v>618</v>
       </c>
@@ -34691,7 +34776,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="33" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
         <v>747</v>
       </c>
@@ -34853,7 +34938,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="34" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
         <v>913</v>
       </c>
@@ -35013,7 +35098,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="35" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
         <v>71</v>
       </c>
@@ -35174,8 +35259,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="BB35" s="9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="36" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
         <v>792</v>
       </c>
@@ -35336,8 +35424,11 @@
         <f t="shared" si="0"/>
         <v>73</v>
       </c>
+      <c r="BB36" s="9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="37" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
         <v>73</v>
       </c>
@@ -35499,7 +35590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>610</v>
       </c>
@@ -35661,7 +35752,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="39" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>866</v>
       </c>
@@ -35823,7 +35914,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="40" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>972</v>
       </c>
@@ -35985,7 +36076,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="41" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>1024</v>
       </c>
@@ -36147,7 +36238,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>1255</v>
       </c>
@@ -36309,7 +36400,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="43" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>1301</v>
       </c>
@@ -36468,7 +36559,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="44" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>75</v>
       </c>
@@ -36630,7 +36721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>215</v>
       </c>
@@ -36792,7 +36883,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="46" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>952</v>
       </c>
@@ -36954,7 +37045,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="47" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>997</v>
       </c>
@@ -37116,7 +37207,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="48" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>1046</v>
       </c>
@@ -37278,7 +37369,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="49" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>1138</v>
       </c>
@@ -37440,7 +37531,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="50" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>1186</v>
       </c>
@@ -37599,7 +37690,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="51" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>77</v>
       </c>
@@ -37761,7 +37852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>139</v>
       </c>
@@ -37923,7 +38014,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="53" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>231</v>
       </c>
@@ -38085,7 +38176,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="54" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>374</v>
       </c>
@@ -38247,7 +38338,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="55" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>501</v>
       </c>
@@ -38409,7 +38500,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="56" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>584</v>
       </c>
@@ -38571,7 +38662,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="57" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>742</v>
       </c>
@@ -38730,7 +38821,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="58" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>79</v>
       </c>
@@ -38892,7 +38983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>164</v>
       </c>
@@ -39054,7 +39145,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="60" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>330</v>
       </c>
@@ -39216,7 +39307,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="61" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>1247</v>
       </c>
@@ -39378,7 +39469,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="62" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>1277</v>
       </c>
@@ -39540,7 +39631,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="63" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>1349</v>
       </c>
@@ -39701,8 +39792,11 @@
         <f t="shared" si="0"/>
         <v>283</v>
       </c>
+      <c r="BB63" s="9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="64" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="5" t="s">
         <v>1574</v>
       </c>
@@ -39862,7 +39956,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="65" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>1487</v>
       </c>
@@ -40021,8 +40115,11 @@
         <f t="shared" si="0"/>
         <v>163</v>
       </c>
+      <c r="BB65" s="9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="66" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="5" t="s">
         <v>1581</v>
       </c>
@@ -40182,7 +40279,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="67" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>81</v>
       </c>
@@ -40344,7 +40441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>964</v>
       </c>
@@ -40506,7 +40603,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="69" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>1075</v>
       </c>
@@ -40668,7 +40765,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="70" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>1270</v>
       </c>
@@ -40830,7 +40927,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="71" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>1334</v>
       </c>
@@ -40992,7 +41089,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="72" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>1388</v>
       </c>
@@ -41154,7 +41251,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="73" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>1411</v>
       </c>
@@ -41313,7 +41410,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="74" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>83</v>
       </c>
@@ -41475,7 +41572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>107</v>
       </c>
@@ -41637,7 +41734,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="76" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>308</v>
       </c>
@@ -41799,7 +41896,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="77" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>670</v>
       </c>
@@ -41961,7 +42058,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="78" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>800</v>
       </c>
@@ -42123,7 +42220,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="79" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>880</v>
       </c>
@@ -42285,7 +42382,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>1063</v>
       </c>
@@ -50202,7 +50299,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="129" spans="1:53" s="16" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:54" s="16" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="16" t="s">
         <v>1109</v>
       </c>
@@ -50360,8 +50457,11 @@
         <f t="shared" si="1"/>
         <v>292</v>
       </c>
+      <c r="BB129" s="16">
+        <v>1</v>
+      </c>
     </row>
-    <row r="130" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>1322</v>
       </c>
@@ -50520,7 +50620,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="131" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>99</v>
       </c>
@@ -50682,7 +50782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>983</v>
       </c>
@@ -50844,7 +50944,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="133" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>1033</v>
       </c>
@@ -51006,7 +51106,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="134" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>1159</v>
       </c>
@@ -51168,7 +51268,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="135" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>1196</v>
       </c>
@@ -51330,7 +51430,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="136" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>1229</v>
       </c>
@@ -51492,7 +51592,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="137" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>1290</v>
       </c>
@@ -51651,7 +51751,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="138" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>101</v>
       </c>
@@ -51813,7 +51913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>1057</v>
       </c>
@@ -51975,7 +52075,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="140" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>1264</v>
       </c>
@@ -52137,7 +52237,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="141" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>1328</v>
       </c>
@@ -52299,7 +52399,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="142" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>1363</v>
       </c>
@@ -52461,7 +52561,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="143" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>1499</v>
       </c>
@@ -52623,7 +52723,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="144" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>1527</v>
       </c>
@@ -55368,7 +55468,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="161" spans="1:53" s="16" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:54" s="16" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="16" t="s">
         <v>1450</v>
       </c>
@@ -55530,7 +55630,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="162" spans="1:53" s="16" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:54" s="16" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="16" t="s">
         <v>1472</v>
       </c>
@@ -55692,7 +55792,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="163" spans="1:53" s="16" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:54" s="16" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="16" t="s">
         <v>1513</v>
       </c>
@@ -55854,7 +55954,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="164" spans="1:53" s="16" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:54" s="16" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="16" t="s">
         <v>1541</v>
       </c>
@@ -56016,7 +56116,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="165" spans="1:53" s="16" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:54" s="16" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="16" t="s">
         <v>1555</v>
       </c>
@@ -56174,8 +56274,11 @@
         <f t="shared" si="2"/>
         <v>336</v>
       </c>
+      <c r="BB165" s="16">
+        <v>1</v>
+      </c>
     </row>
-    <row r="166" spans="1:53" s="16" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:54" s="16" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="16" t="s">
         <v>1567</v>
       </c>
@@ -56334,7 +56437,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="167" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>1288</v>
       </c>
@@ -56496,7 +56599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>1315</v>
       </c>
@@ -56658,7 +56761,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="169" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>1375</v>
       </c>
@@ -56820,7 +56923,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="170" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>1400</v>
       </c>
@@ -56982,7 +57085,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="171" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>1424</v>
       </c>
@@ -57144,7 +57247,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="172" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>1440</v>
       </c>
@@ -57306,7 +57409,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="173" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>1464</v>
       </c>
@@ -57464,8 +57567,11 @@
         <f t="shared" si="2"/>
         <v>64</v>
       </c>
+      <c r="BB173" s="9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="174" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="5" t="s">
         <v>1593</v>
       </c>
@@ -57621,7 +57727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:53" s="20" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:54" s="20" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="5" t="s">
         <v>1601</v>
       </c>
@@ -57779,7 +57885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:53" s="20" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:54" s="20" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="5" t="s">
         <v>1610</v>
       </c>
@@ -58569,18 +58675,10 @@
       <c r="BA180" s="5">
         <v>40</v>
       </c>
-      <c r="BB180" s="5" t="s">
-        <v>728</v>
-      </c>
-      <c r="BC180" s="8" t="s">
-        <v>440</v>
-      </c>
-      <c r="BD180" s="5">
-        <v>0</v>
-      </c>
-      <c r="BE180" s="5">
-        <v>0</v>
-      </c>
+      <c r="BB180" s="5"/>
+      <c r="BC180" s="8"/>
+      <c r="BD180" s="5"/>
+      <c r="BE180" s="5"/>
     </row>
     <row r="181" spans="1:57" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="5" t="s">
@@ -58740,18 +58838,10 @@
       <c r="BA181" s="5">
         <v>13</v>
       </c>
-      <c r="BB181" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="BC181" s="8" t="s">
-        <v>1641</v>
-      </c>
-      <c r="BD181" s="5">
-        <v>0</v>
-      </c>
-      <c r="BE181" s="5">
-        <v>0</v>
-      </c>
+      <c r="BB181" s="5"/>
+      <c r="BC181" s="8"/>
+      <c r="BD181" s="5"/>
+      <c r="BE181" s="5"/>
     </row>
     <row r="182" spans="1:57" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="183" spans="1:57" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>